<commit_message>
refactoring 4th sem code
</commit_message>
<xml_diff>
--- a/Data Science/Advance Excel/Lab 1/1 Introduction of Excel.xlsx
+++ b/Data Science/Advance Excel/Lab 1/1 Introduction of Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Nikhil Vishwakarma\Data Science\Advance Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github repository\Lab-Record\Data Science\Advance Excel\Lab 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768864DB-7141-4447-87A8-EE7890D7DCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4A4418-426F-426E-AD8B-A31AFAD23B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -245,16 +245,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -265,101 +255,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -641,21 +541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="17.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="17.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -711,7 +611,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -722,7 +622,7 @@
         <v>1002</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D25" si="0">_xlfn.CONCAT(B3,C3)</f>
+        <f>_xlfn.CONCAT(B3,C3)</f>
         <v>0187AS221002</v>
       </c>
       <c r="E3" t="s">
@@ -735,7 +635,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -746,7 +646,7 @@
         <v>1003</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B4,C4)</f>
         <v>0187AS221003</v>
       </c>
       <c r="E4" t="s">
@@ -762,7 +662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -773,7 +673,7 @@
         <v>1004</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B5,C5)</f>
         <v>0187AS221004</v>
       </c>
       <c r="E5" t="s">
@@ -792,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -803,7 +703,7 @@
         <v>1005</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B6,C6)</f>
         <v>0187AS221005</v>
       </c>
       <c r="E6" t="s">
@@ -819,7 +719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -830,7 +730,7 @@
         <v>1006</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B7,C7)</f>
         <v>0187AS221006</v>
       </c>
       <c r="E7" t="s">
@@ -846,7 +746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -857,7 +757,7 @@
         <v>1007</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B8,C8)</f>
         <v>0187AS221007</v>
       </c>
       <c r="E8" t="s">
@@ -873,7 +773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -884,7 +784,7 @@
         <v>1008</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B9,C9)</f>
         <v>0187AS221008</v>
       </c>
       <c r="E9" t="s">
@@ -900,7 +800,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -911,7 +811,7 @@
         <v>1009</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B10,C10)</f>
         <v>0187AS221009</v>
       </c>
       <c r="E10" t="s">
@@ -927,7 +827,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -938,7 +838,7 @@
         <v>1010</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B11,C11)</f>
         <v>0187AS221010</v>
       </c>
       <c r="E11" t="s">
@@ -951,7 +851,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -962,7 +862,7 @@
         <v>1011</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B12,C12)</f>
         <v>0187AS221011</v>
       </c>
       <c r="E12" t="s">
@@ -978,7 +878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -989,7 +889,7 @@
         <v>1012</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B13,C13)</f>
         <v>0187AS221012</v>
       </c>
       <c r="E13" t="s">
@@ -1005,7 +905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1016,7 +916,7 @@
         <v>1013</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B14,C14)</f>
         <v>0187AS221013</v>
       </c>
       <c r="E14" t="s">
@@ -1032,7 +932,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1043,7 +943,7 @@
         <v>1014</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B15,C15)</f>
         <v>0187AS221014</v>
       </c>
       <c r="E15" t="s">
@@ -1059,7 +959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1070,7 +970,7 @@
         <v>1015</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B16,C16)</f>
         <v>0187AS221015</v>
       </c>
       <c r="E16" t="s">
@@ -1086,7 +986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1097,7 +997,7 @@
         <v>1016</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B17,C17)</f>
         <v>0187AS221016</v>
       </c>
       <c r="E17" t="s">
@@ -1113,7 +1013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1124,7 +1024,7 @@
         <v>1017</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B18,C18)</f>
         <v>0187AS221017</v>
       </c>
       <c r="E18" t="s">
@@ -1140,7 +1040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1151,7 +1051,7 @@
         <v>1018</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B19,C19)</f>
         <v>0187AS221018</v>
       </c>
       <c r="E19" t="s">
@@ -1167,7 +1067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1178,7 +1078,7 @@
         <v>1019</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B20,C20)</f>
         <v>0187AS221019</v>
       </c>
       <c r="E20" t="s">
@@ -1194,7 +1094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1205,7 +1105,7 @@
         <v>1020</v>
       </c>
       <c r="D21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B21,C21)</f>
         <v>0187AS221020</v>
       </c>
       <c r="E21" t="s">
@@ -1221,7 +1121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1232,7 +1132,7 @@
         <v>1021</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B22,C22)</f>
         <v>0187AS221021</v>
       </c>
       <c r="E22" t="s">
@@ -1248,7 +1148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1259,7 +1159,7 @@
         <v>1022</v>
       </c>
       <c r="D23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B23,C23)</f>
         <v>0187AS221022</v>
       </c>
       <c r="E23" t="s">
@@ -1272,7 +1172,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1283,7 +1183,7 @@
         <v>1023</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B24,C24)</f>
         <v>0187AS221023</v>
       </c>
       <c r="E24" t="s">
@@ -1296,7 +1196,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1307,7 +1207,7 @@
         <v>1024</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B25,C25)</f>
         <v>0187AS221024</v>
       </c>
       <c r="E25" t="s">
@@ -1320,28 +1220,35 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I26" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I27" s="3">
         <f>SUM(H2:H26)</f>
         <v>3688</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576 L1:L1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
-    <cfRule type="uniqueValues" dxfId="7" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1 E1:E1048576 L1:L1048576">
+    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ohho" error="gfg" promptTitle="hi" prompt="dood" sqref="O26" xr:uid="{7B5B1DFE-1692-4ADE-8C60-A2EF7149A2DC}">
+      <formula1>1</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>